<commit_message>
- Update Data Prolific - Regression Model Adjustment (Adding controls and moderation) - Rework Workflow Prolific Data
</commit_message>
<xml_diff>
--- a/Data_EE Downward Causation_Conjoint_Prolific.xlsx
+++ b/Data_EE Downward Causation_Conjoint_Prolific.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johannes.haehnlein\Desktop\Johannes Haehnlein\19_PROMOTION\01_STUDIEN\Studie 2 - Conjoint\Data\R Repository\EE_Downward-Causation_Entrepreneurship-Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F00D961A-7AD4-4FC9-B4FB-2C548DB74B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102377BF-EB23-4EEE-B559-EDE4367DD6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Sudoku</t>
-  </si>
-  <si>
-    <t>interviewtime</t>
   </si>
   <si>
     <t>Berlin</t>
@@ -550,6 +547,9 @@
   <si>
     <t>GenTrust6</t>
   </si>
+  <si>
+    <t>duration</t>
+  </si>
 </sst>
 </file>
 
@@ -904,7 +904,7 @@
   <dimension ref="A1:BZ183"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection sqref="A1:BZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -915,239 +915,239 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:78" x14ac:dyDescent="0.25">
@@ -1179,7 +1179,7 @@
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2">
         <v>30</v>
@@ -1415,7 +1415,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1651,7 +1651,7 @@
         <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1887,7 +1887,7 @@
         <v>9</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5">
         <v>10</v>
@@ -2123,7 +2123,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -2359,7 +2359,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7">
         <v>8</v>
@@ -2595,7 +2595,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -2831,7 +2831,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -3067,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -3300,7 +3300,7 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -3536,7 +3536,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K12">
         <v>500</v>
@@ -3769,7 +3769,7 @@
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K13">
         <v>2</v>
@@ -4005,7 +4005,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -4241,7 +4241,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K15">
         <v>3</v>
@@ -4477,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K16">
         <v>2</v>
@@ -4713,7 +4713,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K17">
         <v>2</v>
@@ -4949,7 +4949,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -5185,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -5421,7 +5421,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -5657,7 +5657,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -5893,7 +5893,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -6129,7 +6129,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -6365,7 +6365,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K24">
         <v>3</v>
@@ -6601,7 +6601,7 @@
         <v>6</v>
       </c>
       <c r="J25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K25">
         <v>2</v>
@@ -6837,7 +6837,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -7073,7 +7073,7 @@
         <v>9</v>
       </c>
       <c r="J27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -7309,7 +7309,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -7545,7 +7545,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -7781,7 +7781,7 @@
         <v>7</v>
       </c>
       <c r="J30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K30">
         <v>63</v>
@@ -8014,7 +8014,7 @@
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K31">
         <v>2</v>
@@ -8250,7 +8250,7 @@
         <v>3</v>
       </c>
       <c r="J32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K32">
         <v>50</v>
@@ -8483,7 +8483,7 @@
         <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K33">
         <v>27</v>
@@ -8719,7 +8719,7 @@
         <v>9</v>
       </c>
       <c r="J34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K34">
         <v>3</v>
@@ -8955,7 +8955,7 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -9191,7 +9191,7 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K36">
         <v>1</v>
@@ -9424,7 +9424,7 @@
         <v>2</v>
       </c>
       <c r="J37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K37">
         <v>22</v>
@@ -9660,7 +9660,7 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K38">
         <v>1</v>
@@ -9896,7 +9896,7 @@
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -10129,7 +10129,7 @@
         <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K40">
         <v>3</v>
@@ -10365,7 +10365,7 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -10598,7 +10598,7 @@
         <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K42">
         <v>3</v>
@@ -10834,7 +10834,7 @@
         <v>9</v>
       </c>
       <c r="J43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -11070,7 +11070,7 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K44">
         <v>1</v>
@@ -11306,7 +11306,7 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K45">
         <v>50</v>
@@ -11542,7 +11542,7 @@
         <v>9</v>
       </c>
       <c r="J46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -11775,7 +11775,7 @@
         <v>2</v>
       </c>
       <c r="J47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K47">
         <v>4</v>
@@ -12011,7 +12011,7 @@
         <v>7</v>
       </c>
       <c r="J48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K48">
         <v>10000</v>
@@ -12247,7 +12247,7 @@
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K49">
         <v>3</v>
@@ -12483,7 +12483,7 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K50">
         <v>1</v>
@@ -12719,7 +12719,7 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K51">
         <v>5</v>
@@ -12955,7 +12955,7 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K52">
         <v>2</v>
@@ -13191,7 +13191,7 @@
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -13424,7 +13424,7 @@
         <v>2</v>
       </c>
       <c r="J54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K54">
         <v>1</v>
@@ -13660,7 +13660,7 @@
         <v>2</v>
       </c>
       <c r="J55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K55">
         <v>3</v>
@@ -13896,7 +13896,7 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K56">
         <v>1</v>
@@ -14132,7 +14132,7 @@
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -14368,7 +14368,7 @@
         <v>1</v>
       </c>
       <c r="J58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -14604,7 +14604,7 @@
         <v>6</v>
       </c>
       <c r="J59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K59">
         <v>3</v>
@@ -14837,7 +14837,7 @@
         <v>2</v>
       </c>
       <c r="J60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K60">
         <v>1</v>
@@ -15073,7 +15073,7 @@
         <v>6</v>
       </c>
       <c r="J61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K61">
         <v>1</v>
@@ -15309,7 +15309,7 @@
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K62">
         <v>1</v>
@@ -15545,7 +15545,7 @@
         <v>1</v>
       </c>
       <c r="J63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K63">
         <v>3</v>
@@ -15781,7 +15781,7 @@
         <v>1</v>
       </c>
       <c r="J64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -16017,7 +16017,7 @@
         <v>9</v>
       </c>
       <c r="J65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K65">
         <v>0</v>
@@ -16253,7 +16253,7 @@
         <v>1</v>
       </c>
       <c r="J66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -16486,7 +16486,7 @@
         <v>2</v>
       </c>
       <c r="J67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K67">
         <v>15</v>
@@ -16722,7 +16722,7 @@
         <v>1</v>
       </c>
       <c r="J68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K68">
         <v>0</v>
@@ -16958,7 +16958,7 @@
         <v>1</v>
       </c>
       <c r="J69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K69">
         <v>2</v>
@@ -17194,7 +17194,7 @@
         <v>6</v>
       </c>
       <c r="J70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K70">
         <v>1</v>
@@ -17430,7 +17430,7 @@
         <v>6</v>
       </c>
       <c r="J71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K71">
         <v>1</v>
@@ -17666,7 +17666,7 @@
         <v>1</v>
       </c>
       <c r="J72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K72">
         <v>2</v>
@@ -17899,7 +17899,7 @@
         <v>2</v>
       </c>
       <c r="J73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K73">
         <v>4500</v>
@@ -18135,7 +18135,7 @@
         <v>1</v>
       </c>
       <c r="J74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K74">
         <v>1</v>
@@ -18368,7 +18368,7 @@
         <v>2</v>
       </c>
       <c r="J75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K75">
         <v>2</v>
@@ -18604,7 +18604,7 @@
         <v>1</v>
       </c>
       <c r="J76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K76">
         <v>15</v>
@@ -18840,7 +18840,7 @@
         <v>1</v>
       </c>
       <c r="J77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K77">
         <v>3</v>
@@ -19076,7 +19076,7 @@
         <v>1</v>
       </c>
       <c r="J78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K78">
         <v>1</v>
@@ -19312,7 +19312,7 @@
         <v>7</v>
       </c>
       <c r="J79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K79">
         <v>23</v>
@@ -19548,7 +19548,7 @@
         <v>1</v>
       </c>
       <c r="J80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K80">
         <v>1</v>
@@ -19784,7 +19784,7 @@
         <v>1</v>
       </c>
       <c r="J81" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K81">
         <v>1</v>
@@ -20020,7 +20020,7 @@
         <v>1</v>
       </c>
       <c r="J82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K82">
         <v>1</v>
@@ -20256,7 +20256,7 @@
         <v>1</v>
       </c>
       <c r="J83" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K83">
         <v>2</v>
@@ -20492,7 +20492,7 @@
         <v>1</v>
       </c>
       <c r="J84" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K84">
         <v>1</v>
@@ -20728,7 +20728,7 @@
         <v>9</v>
       </c>
       <c r="J85" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K85">
         <v>1</v>
@@ -20964,7 +20964,7 @@
         <v>4</v>
       </c>
       <c r="J86" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K86">
         <v>55</v>
@@ -21197,7 +21197,7 @@
         <v>2</v>
       </c>
       <c r="J87" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K87">
         <v>5</v>
@@ -21433,7 +21433,7 @@
         <v>1</v>
       </c>
       <c r="J88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K88">
         <v>2</v>
@@ -21669,7 +21669,7 @@
         <v>1</v>
       </c>
       <c r="J89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K89">
         <v>2</v>
@@ -21905,7 +21905,7 @@
         <v>6</v>
       </c>
       <c r="J90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -22141,7 +22141,7 @@
         <v>1</v>
       </c>
       <c r="J91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K91">
         <v>60</v>
@@ -22377,7 +22377,7 @@
         <v>1</v>
       </c>
       <c r="J92" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K92">
         <v>2</v>
@@ -22613,7 +22613,7 @@
         <v>1</v>
       </c>
       <c r="J93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K93">
         <v>5</v>
@@ -22849,7 +22849,7 @@
         <v>1</v>
       </c>
       <c r="J94" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -23082,7 +23082,7 @@
         <v>2</v>
       </c>
       <c r="J95" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K95">
         <v>3</v>
@@ -23318,7 +23318,7 @@
         <v>1</v>
       </c>
       <c r="J96" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K96">
         <v>0</v>
@@ -23551,7 +23551,7 @@
         <v>2</v>
       </c>
       <c r="J97" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K97">
         <v>1</v>
@@ -23787,7 +23787,7 @@
         <v>1</v>
       </c>
       <c r="J98" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K98">
         <v>3</v>
@@ -24023,7 +24023,7 @@
         <v>6</v>
       </c>
       <c r="J99" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K99">
         <v>3</v>
@@ -24259,7 +24259,7 @@
         <v>1</v>
       </c>
       <c r="J100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K100">
         <v>1</v>
@@ -24495,7 +24495,7 @@
         <v>1</v>
       </c>
       <c r="J101" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K101">
         <v>1</v>
@@ -24731,7 +24731,7 @@
         <v>1</v>
       </c>
       <c r="J102" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K102">
         <v>1</v>
@@ -24967,7 +24967,7 @@
         <v>1</v>
       </c>
       <c r="J103" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K103">
         <v>1</v>
@@ -25200,7 +25200,7 @@
         <v>2</v>
       </c>
       <c r="J104" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K104">
         <v>6</v>
@@ -25436,7 +25436,7 @@
         <v>1</v>
       </c>
       <c r="J105" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K105">
         <v>5</v>
@@ -25672,7 +25672,7 @@
         <v>1</v>
       </c>
       <c r="J106" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K106">
         <v>1</v>
@@ -25908,7 +25908,7 @@
         <v>1</v>
       </c>
       <c r="J107" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K107">
         <v>3</v>
@@ -26144,7 +26144,7 @@
         <v>1</v>
       </c>
       <c r="J108" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K108">
         <v>1</v>
@@ -26380,7 +26380,7 @@
         <v>6</v>
       </c>
       <c r="J109" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K109">
         <v>2</v>
@@ -26616,7 +26616,7 @@
         <v>1</v>
       </c>
       <c r="J110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K110">
         <v>0</v>
@@ -26849,7 +26849,7 @@
         <v>2</v>
       </c>
       <c r="J111" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K111">
         <v>5</v>
@@ -27085,7 +27085,7 @@
         <v>1</v>
       </c>
       <c r="J112" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K112">
         <v>0</v>
@@ -27321,7 +27321,7 @@
         <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K113">
         <v>1</v>
@@ -27557,7 +27557,7 @@
         <v>1</v>
       </c>
       <c r="J114" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K114">
         <v>1</v>
@@ -27790,7 +27790,7 @@
         <v>2</v>
       </c>
       <c r="J115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K115">
         <v>1</v>
@@ -28026,7 +28026,7 @@
         <v>1</v>
       </c>
       <c r="J116" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K116">
         <v>1</v>
@@ -28262,7 +28262,7 @@
         <v>1</v>
       </c>
       <c r="J117" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K117">
         <v>1</v>
@@ -28498,7 +28498,7 @@
         <v>1</v>
       </c>
       <c r="J118" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K118">
         <v>0</v>
@@ -28734,7 +28734,7 @@
         <v>1</v>
       </c>
       <c r="J119" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K119">
         <v>1</v>
@@ -28970,7 +28970,7 @@
         <v>1</v>
       </c>
       <c r="J120" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K120">
         <v>1</v>
@@ -29206,7 +29206,7 @@
         <v>1</v>
       </c>
       <c r="J121" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K121">
         <v>1</v>
@@ -29442,7 +29442,7 @@
         <v>1</v>
       </c>
       <c r="J122" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K122">
         <v>1</v>
@@ -29678,7 +29678,7 @@
         <v>1</v>
       </c>
       <c r="J123" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K123">
         <v>2</v>
@@ -29914,7 +29914,7 @@
         <v>1</v>
       </c>
       <c r="J124" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K124">
         <v>1</v>
@@ -30150,7 +30150,7 @@
         <v>9</v>
       </c>
       <c r="J125" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K125">
         <v>12</v>
@@ -30386,7 +30386,7 @@
         <v>1</v>
       </c>
       <c r="J126" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K126">
         <v>1</v>
@@ -30619,7 +30619,7 @@
         <v>2</v>
       </c>
       <c r="J127" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K127">
         <v>5</v>
@@ -30855,7 +30855,7 @@
         <v>1</v>
       </c>
       <c r="J128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K128">
         <v>1</v>
@@ -31088,7 +31088,7 @@
         <v>2</v>
       </c>
       <c r="J129" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K129">
         <v>2</v>
@@ -31324,7 +31324,7 @@
         <v>1</v>
       </c>
       <c r="J130" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K130">
         <v>3</v>
@@ -31560,7 +31560,7 @@
         <v>9</v>
       </c>
       <c r="J131" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K131">
         <v>0</v>
@@ -31796,7 +31796,7 @@
         <v>1</v>
       </c>
       <c r="J132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K132">
         <v>2</v>
@@ -32032,7 +32032,7 @@
         <v>1</v>
       </c>
       <c r="J133" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K133">
         <v>5</v>
@@ -32268,7 +32268,7 @@
         <v>1</v>
       </c>
       <c r="J134" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K134">
         <v>2</v>
@@ -32504,7 +32504,7 @@
         <v>1</v>
       </c>
       <c r="J135" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K135">
         <v>1</v>
@@ -32740,7 +32740,7 @@
         <v>9</v>
       </c>
       <c r="J136" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K136">
         <v>2</v>
@@ -32976,7 +32976,7 @@
         <v>1</v>
       </c>
       <c r="J137" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K137">
         <v>1</v>
@@ -33212,7 +33212,7 @@
         <v>1</v>
       </c>
       <c r="J138" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K138">
         <v>1</v>
@@ -33448,7 +33448,7 @@
         <v>1</v>
       </c>
       <c r="J139" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K139">
         <v>1</v>
@@ -33684,7 +33684,7 @@
         <v>1</v>
       </c>
       <c r="J140" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K140">
         <v>1</v>
@@ -33920,7 +33920,7 @@
         <v>1</v>
       </c>
       <c r="J141" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K141">
         <v>1</v>
@@ -34153,7 +34153,7 @@
         <v>2</v>
       </c>
       <c r="J142" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K142">
         <v>2</v>
@@ -34389,7 +34389,7 @@
         <v>1</v>
       </c>
       <c r="J143" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K143">
         <v>2</v>
@@ -34625,7 +34625,7 @@
         <v>1</v>
       </c>
       <c r="J144" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K144">
         <v>1</v>
@@ -34861,7 +34861,7 @@
         <v>1</v>
       </c>
       <c r="J145" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K145">
         <v>3</v>
@@ -35097,7 +35097,7 @@
         <v>1</v>
       </c>
       <c r="J146" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K146">
         <v>1</v>
@@ -35333,7 +35333,7 @@
         <v>1</v>
       </c>
       <c r="J147" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K147">
         <v>1</v>
@@ -35569,7 +35569,7 @@
         <v>1</v>
       </c>
       <c r="J148" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K148">
         <v>1</v>
@@ -35805,7 +35805,7 @@
         <v>1</v>
       </c>
       <c r="J149" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K149">
         <v>5</v>
@@ -36041,7 +36041,7 @@
         <v>1</v>
       </c>
       <c r="J150" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K150">
         <v>3</v>
@@ -36277,7 +36277,7 @@
         <v>6</v>
       </c>
       <c r="J151" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K151">
         <v>2</v>
@@ -36513,7 +36513,7 @@
         <v>9</v>
       </c>
       <c r="J152" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K152">
         <v>3</v>
@@ -36749,7 +36749,7 @@
         <v>1</v>
       </c>
       <c r="J153" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K153">
         <v>1</v>
@@ -36982,7 +36982,7 @@
         <v>2</v>
       </c>
       <c r="J154" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K154">
         <v>19</v>
@@ -37218,7 +37218,7 @@
         <v>1</v>
       </c>
       <c r="J155" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K155">
         <v>1</v>
@@ -37451,7 +37451,7 @@
         <v>2</v>
       </c>
       <c r="J156" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K156">
         <v>100</v>
@@ -37687,7 +37687,7 @@
         <v>1</v>
       </c>
       <c r="J157" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K157">
         <v>1</v>
@@ -37923,7 +37923,7 @@
         <v>9</v>
       </c>
       <c r="J158" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K158">
         <v>1</v>
@@ -38156,7 +38156,7 @@
         <v>2</v>
       </c>
       <c r="J159" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K159">
         <v>2</v>
@@ -38392,7 +38392,7 @@
         <v>1</v>
       </c>
       <c r="J160" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K160">
         <v>1</v>
@@ -38628,7 +38628,7 @@
         <v>1</v>
       </c>
       <c r="J161" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K161">
         <v>1</v>
@@ -38864,7 +38864,7 @@
         <v>1</v>
       </c>
       <c r="J162" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K162">
         <v>1</v>
@@ -39100,7 +39100,7 @@
         <v>9</v>
       </c>
       <c r="J163" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K163">
         <v>5</v>
@@ -39336,7 +39336,7 @@
         <v>1</v>
       </c>
       <c r="J164" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K164">
         <v>1</v>
@@ -39572,7 +39572,7 @@
         <v>9</v>
       </c>
       <c r="J165" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K165">
         <v>1</v>
@@ -39808,7 +39808,7 @@
         <v>1</v>
       </c>
       <c r="J166" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K166">
         <v>1</v>
@@ -40041,7 +40041,7 @@
         <v>2</v>
       </c>
       <c r="J167" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K167">
         <v>0</v>
@@ -40277,7 +40277,7 @@
         <v>1</v>
       </c>
       <c r="J168" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K168">
         <v>1</v>
@@ -40510,7 +40510,7 @@
         <v>2</v>
       </c>
       <c r="J169" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K169">
         <v>8</v>
@@ -40746,7 +40746,7 @@
         <v>1</v>
       </c>
       <c r="J170" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K170">
         <v>5</v>
@@ -40982,7 +40982,7 @@
         <v>9</v>
       </c>
       <c r="J171" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K171">
         <v>0</v>
@@ -41218,7 +41218,7 @@
         <v>1</v>
       </c>
       <c r="J172" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K172">
         <v>0</v>
@@ -41454,7 +41454,7 @@
         <v>1</v>
       </c>
       <c r="J173" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K173">
         <v>1</v>
@@ -41687,7 +41687,7 @@
         <v>2</v>
       </c>
       <c r="J174" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K174">
         <v>5</v>
@@ -41920,7 +41920,7 @@
         <v>2</v>
       </c>
       <c r="J175" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K175">
         <v>1</v>
@@ -42156,7 +42156,7 @@
         <v>1</v>
       </c>
       <c r="J176" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K176">
         <v>2</v>
@@ -42392,7 +42392,7 @@
         <v>9</v>
       </c>
       <c r="J177" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K177">
         <v>7</v>
@@ -42628,7 +42628,7 @@
         <v>1</v>
       </c>
       <c r="J178" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K178">
         <v>7</v>
@@ -42864,7 +42864,7 @@
         <v>1</v>
       </c>
       <c r="J179" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K179">
         <v>0</v>
@@ -43100,7 +43100,7 @@
         <v>1</v>
       </c>
       <c r="J180" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K180">
         <v>1</v>
@@ -43336,7 +43336,7 @@
         <v>9</v>
       </c>
       <c r="J181" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K181">
         <v>1</v>
@@ -43569,7 +43569,7 @@
         <v>2</v>
       </c>
       <c r="J182" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K182">
         <v>2</v>
@@ -43802,7 +43802,7 @@
         <v>2</v>
       </c>
       <c r="J183" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K183">
         <v>1</v>

</xml_diff>

<commit_message>
- adding data set comparison
</commit_message>
<xml_diff>
--- a/Data_EE Downward Causation_Conjoint_Prolific.xlsx
+++ b/Data_EE Downward Causation_Conjoint_Prolific.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johannes.haehnlein\Desktop\Johannes Haehnlein\19_PROMOTION\01_STUDIEN\Studie 2 - Conjoint\Data\R Repository\EE_Downward-Causation_Entrepreneurship-Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102377BF-EB23-4EEE-B559-EDE4367DD6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8310A343-C835-4E1F-99DF-90125103F53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studie zur Stärkung von Gründun" sheetId="1" r:id="rId1"/>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BZ183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:BZ1"/>
+    <sheetView tabSelected="1" topLeftCell="H162" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N183" sqref="L2:N183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <v>6</v>
@@ -1421,13 +1421,13 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>6</v>
@@ -1657,13 +1657,13 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>6</v>
@@ -1893,13 +1893,13 @@
         <v>10</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <v>6</v>
@@ -2129,13 +2129,13 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <v>6</v>
@@ -2365,13 +2365,13 @@
         <v>8</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>6</v>
@@ -2601,13 +2601,13 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>6</v>
@@ -2837,13 +2837,13 @@
         <v>2</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>6</v>
@@ -3073,13 +3073,13 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>6</v>
@@ -3306,13 +3306,13 @@
         <v>2</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <v>6</v>
@@ -3775,13 +3775,13 @@
         <v>2</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O13">
         <v>6</v>
@@ -4011,13 +4011,13 @@
         <v>1</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O14">
         <v>6</v>
@@ -4247,13 +4247,13 @@
         <v>3</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O15">
         <v>6</v>
@@ -4483,13 +4483,13 @@
         <v>2</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O16">
         <v>6</v>
@@ -4719,13 +4719,13 @@
         <v>2</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O17">
         <v>6</v>
@@ -4958,10 +4958,10 @@
         <v>1</v>
       </c>
       <c r="M18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O18">
         <v>6</v>
@@ -5191,13 +5191,13 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <v>6</v>
@@ -5427,13 +5427,13 @@
         <v>1</v>
       </c>
       <c r="L20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O20">
         <v>6</v>
@@ -5663,13 +5663,13 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O21">
         <v>6</v>
@@ -5899,13 +5899,13 @@
         <v>1</v>
       </c>
       <c r="L22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <v>6</v>
@@ -6135,13 +6135,13 @@
         <v>1</v>
       </c>
       <c r="L23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O23">
         <v>6</v>
@@ -6371,13 +6371,13 @@
         <v>3</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O24">
         <v>6</v>
@@ -6607,13 +6607,13 @@
         <v>2</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O25">
         <v>6</v>
@@ -6843,13 +6843,13 @@
         <v>1</v>
       </c>
       <c r="L26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O26">
         <v>6</v>
@@ -7079,13 +7079,13 @@
         <v>1</v>
       </c>
       <c r="L27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O27">
         <v>6</v>
@@ -7315,13 +7315,13 @@
         <v>1</v>
       </c>
       <c r="L28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O28">
         <v>6</v>
@@ -7554,10 +7554,10 @@
         <v>1</v>
       </c>
       <c r="M29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O29">
         <v>6</v>
@@ -7787,13 +7787,13 @@
         <v>63</v>
       </c>
       <c r="L30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O30">
         <v>6</v>
@@ -8020,13 +8020,13 @@
         <v>2</v>
       </c>
       <c r="L31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O31">
         <v>6</v>
@@ -8256,13 +8256,13 @@
         <v>50</v>
       </c>
       <c r="L32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O32">
         <v>6</v>
@@ -8489,13 +8489,13 @@
         <v>27</v>
       </c>
       <c r="L33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O33">
         <v>6</v>
@@ -8725,13 +8725,13 @@
         <v>3</v>
       </c>
       <c r="L34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O34">
         <v>6</v>
@@ -8961,13 +8961,13 @@
         <v>1</v>
       </c>
       <c r="L35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O35">
         <v>6</v>
@@ -9197,13 +9197,13 @@
         <v>1</v>
       </c>
       <c r="L36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O36">
         <v>6</v>
@@ -9430,13 +9430,13 @@
         <v>22</v>
       </c>
       <c r="L37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O37">
         <v>6</v>
@@ -9666,13 +9666,13 @@
         <v>1</v>
       </c>
       <c r="L38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O38">
         <v>6</v>
@@ -9902,13 +9902,13 @@
         <v>1</v>
       </c>
       <c r="L39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O39">
         <v>6</v>
@@ -10135,10 +10135,10 @@
         <v>3</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N40">
         <v>1</v>
@@ -10371,13 +10371,13 @@
         <v>0</v>
       </c>
       <c r="L41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O41">
         <v>6</v>
@@ -10604,7 +10604,7 @@
         <v>3</v>
       </c>
       <c r="L42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M42">
         <v>1</v>
@@ -10843,10 +10843,10 @@
         <v>1</v>
       </c>
       <c r="M43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O43">
         <v>6</v>
@@ -11076,10 +11076,10 @@
         <v>1</v>
       </c>
       <c r="L44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N44">
         <v>1</v>
@@ -11315,10 +11315,10 @@
         <v>1</v>
       </c>
       <c r="M45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O45">
         <v>6</v>
@@ -11548,13 +11548,13 @@
         <v>0</v>
       </c>
       <c r="L46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O46">
         <v>6</v>
@@ -11781,13 +11781,13 @@
         <v>4</v>
       </c>
       <c r="L47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M47">
         <v>1</v>
       </c>
       <c r="N47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O47">
         <v>6</v>
@@ -12017,13 +12017,13 @@
         <v>10000</v>
       </c>
       <c r="L48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O48">
         <v>6</v>
@@ -12253,13 +12253,13 @@
         <v>3</v>
       </c>
       <c r="L49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O49">
         <v>6</v>
@@ -12489,13 +12489,13 @@
         <v>1</v>
       </c>
       <c r="L50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O50">
         <v>6</v>
@@ -12725,13 +12725,13 @@
         <v>5</v>
       </c>
       <c r="L51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O51">
         <v>6</v>
@@ -12961,13 +12961,13 @@
         <v>2</v>
       </c>
       <c r="L52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O52">
         <v>6</v>
@@ -13197,13 +13197,13 @@
         <v>0</v>
       </c>
       <c r="L53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O53">
         <v>6</v>
@@ -13430,13 +13430,13 @@
         <v>1</v>
       </c>
       <c r="L54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O54">
         <v>6</v>
@@ -13669,7 +13669,7 @@
         <v>1</v>
       </c>
       <c r="M55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -13902,13 +13902,13 @@
         <v>1</v>
       </c>
       <c r="L56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O56">
         <v>6</v>
@@ -14138,13 +14138,13 @@
         <v>0</v>
       </c>
       <c r="L57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O57">
         <v>6</v>
@@ -14610,13 +14610,13 @@
         <v>3</v>
       </c>
       <c r="L59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O59">
         <v>6</v>
@@ -14843,13 +14843,13 @@
         <v>1</v>
       </c>
       <c r="L60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O60">
         <v>6</v>
@@ -15079,13 +15079,13 @@
         <v>1</v>
       </c>
       <c r="L61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O61">
         <v>6</v>
@@ -15315,13 +15315,13 @@
         <v>1</v>
       </c>
       <c r="L62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O62">
         <v>6</v>
@@ -15551,13 +15551,13 @@
         <v>3</v>
       </c>
       <c r="L63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O63">
         <v>6</v>
@@ -15787,13 +15787,13 @@
         <v>1</v>
       </c>
       <c r="L64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O64">
         <v>6</v>
@@ -16023,13 +16023,13 @@
         <v>0</v>
       </c>
       <c r="L65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O65">
         <v>6</v>
@@ -16259,13 +16259,13 @@
         <v>1</v>
       </c>
       <c r="L66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O66">
         <v>6</v>
@@ -16492,13 +16492,13 @@
         <v>15</v>
       </c>
       <c r="L67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O67">
         <v>6</v>
@@ -16728,13 +16728,13 @@
         <v>0</v>
       </c>
       <c r="L68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O68">
         <v>6</v>
@@ -16964,13 +16964,13 @@
         <v>2</v>
       </c>
       <c r="L69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O69">
         <v>6</v>
@@ -17200,13 +17200,13 @@
         <v>1</v>
       </c>
       <c r="L70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O70">
         <v>6</v>
@@ -17436,13 +17436,13 @@
         <v>1</v>
       </c>
       <c r="L71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O71">
         <v>6</v>
@@ -17672,13 +17672,13 @@
         <v>2</v>
       </c>
       <c r="L72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O72">
         <v>6</v>
@@ -17905,10 +17905,10 @@
         <v>4500</v>
       </c>
       <c r="L73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N73">
         <v>1</v>
@@ -18141,13 +18141,13 @@
         <v>1</v>
       </c>
       <c r="L74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O74">
         <v>6</v>
@@ -18374,13 +18374,13 @@
         <v>2</v>
       </c>
       <c r="L75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O75">
         <v>6</v>
@@ -18610,13 +18610,13 @@
         <v>15</v>
       </c>
       <c r="L76">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N76">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O76">
         <v>6</v>
@@ -18846,13 +18846,13 @@
         <v>3</v>
       </c>
       <c r="L77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O77">
         <v>6</v>
@@ -19082,13 +19082,13 @@
         <v>1</v>
       </c>
       <c r="L78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O78">
         <v>6</v>
@@ -19321,7 +19321,7 @@
         <v>1</v>
       </c>
       <c r="M79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N79">
         <v>1</v>
@@ -19554,13 +19554,13 @@
         <v>1</v>
       </c>
       <c r="L80">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O80">
         <v>6</v>
@@ -19790,13 +19790,13 @@
         <v>1</v>
       </c>
       <c r="L81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O81">
         <v>6</v>
@@ -20026,13 +20026,13 @@
         <v>1</v>
       </c>
       <c r="L82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M82">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N82">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O82">
         <v>6</v>
@@ -20262,13 +20262,13 @@
         <v>2</v>
       </c>
       <c r="L83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O83">
         <v>6</v>
@@ -20498,13 +20498,13 @@
         <v>1</v>
       </c>
       <c r="L84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M84">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N84">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O84">
         <v>6</v>
@@ -20734,13 +20734,13 @@
         <v>1</v>
       </c>
       <c r="L85">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M85">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O85">
         <v>6</v>
@@ -21203,13 +21203,13 @@
         <v>5</v>
       </c>
       <c r="L87">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M87">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N87">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O87">
         <v>6</v>
@@ -21439,13 +21439,13 @@
         <v>2</v>
       </c>
       <c r="L88">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O88">
         <v>6</v>
@@ -21675,10 +21675,10 @@
         <v>2</v>
       </c>
       <c r="L89">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M89">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N89">
         <v>1</v>
@@ -21911,13 +21911,13 @@
         <v>1</v>
       </c>
       <c r="L90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M90">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N90">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O90">
         <v>6</v>
@@ -22150,10 +22150,10 @@
         <v>1</v>
       </c>
       <c r="M91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N91">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O91">
         <v>6</v>
@@ -22383,13 +22383,13 @@
         <v>2</v>
       </c>
       <c r="L92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O92">
         <v>6</v>
@@ -22619,13 +22619,13 @@
         <v>5</v>
       </c>
       <c r="L93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N93">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O93">
         <v>6</v>
@@ -22855,13 +22855,13 @@
         <v>1</v>
       </c>
       <c r="L94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M94">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N94">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O94">
         <v>6</v>
@@ -23088,7 +23088,7 @@
         <v>3</v>
       </c>
       <c r="L95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M95">
         <v>1</v>
@@ -23557,13 +23557,13 @@
         <v>1</v>
       </c>
       <c r="L97">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M97">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O97">
         <v>6</v>
@@ -23793,13 +23793,13 @@
         <v>3</v>
       </c>
       <c r="L98">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M98">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N98">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O98">
         <v>6</v>
@@ -24029,13 +24029,13 @@
         <v>3</v>
       </c>
       <c r="L99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M99">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N99">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O99">
         <v>6</v>
@@ -24265,13 +24265,13 @@
         <v>1</v>
       </c>
       <c r="L100">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M100">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N100">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O100">
         <v>6</v>
@@ -24501,13 +24501,13 @@
         <v>1</v>
       </c>
       <c r="L101">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M101">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O101">
         <v>6</v>
@@ -24737,13 +24737,13 @@
         <v>1</v>
       </c>
       <c r="L102">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M102">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N102">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O102">
         <v>6</v>
@@ -24973,13 +24973,13 @@
         <v>1</v>
       </c>
       <c r="L103">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N103">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O103">
         <v>6</v>
@@ -25206,13 +25206,13 @@
         <v>6</v>
       </c>
       <c r="L104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O104">
         <v>6</v>
@@ -25442,13 +25442,13 @@
         <v>5</v>
       </c>
       <c r="L105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O105">
         <v>6</v>
@@ -25678,13 +25678,13 @@
         <v>1</v>
       </c>
       <c r="L106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M106">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O106">
         <v>6</v>
@@ -25914,13 +25914,13 @@
         <v>3</v>
       </c>
       <c r="L107">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N107">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O107">
         <v>6</v>
@@ -26150,13 +26150,13 @@
         <v>1</v>
       </c>
       <c r="L108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M108">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N108">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O108">
         <v>6</v>
@@ -26386,13 +26386,13 @@
         <v>2</v>
       </c>
       <c r="L109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O109">
         <v>6</v>
@@ -26622,13 +26622,13 @@
         <v>0</v>
       </c>
       <c r="L110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M110">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N110">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O110">
         <v>6</v>
@@ -26855,7 +26855,7 @@
         <v>5</v>
       </c>
       <c r="L111">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M111">
         <v>1</v>
@@ -27091,13 +27091,13 @@
         <v>0</v>
       </c>
       <c r="L112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O112">
         <v>6</v>
@@ -27327,13 +27327,13 @@
         <v>1</v>
       </c>
       <c r="L113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O113">
         <v>6</v>
@@ -27563,13 +27563,13 @@
         <v>1</v>
       </c>
       <c r="L114">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M114">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N114">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O114">
         <v>6</v>
@@ -27796,13 +27796,13 @@
         <v>1</v>
       </c>
       <c r="L115">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M115">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N115">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O115">
         <v>6</v>
@@ -28032,13 +28032,13 @@
         <v>1</v>
       </c>
       <c r="L116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M116">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N116">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O116">
         <v>6</v>
@@ -28268,13 +28268,13 @@
         <v>1</v>
       </c>
       <c r="L117">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M117">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N117">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O117">
         <v>6</v>
@@ -28504,13 +28504,13 @@
         <v>0</v>
       </c>
       <c r="L118">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M118">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N118">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O118">
         <v>6</v>
@@ -28740,13 +28740,13 @@
         <v>1</v>
       </c>
       <c r="L119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O119">
         <v>6</v>
@@ -28976,13 +28976,13 @@
         <v>1</v>
       </c>
       <c r="L120">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M120">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N120">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O120">
         <v>6</v>
@@ -29212,13 +29212,13 @@
         <v>1</v>
       </c>
       <c r="L121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M121">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N121">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O121">
         <v>6</v>
@@ -29448,13 +29448,13 @@
         <v>1</v>
       </c>
       <c r="L122">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O122">
         <v>6</v>
@@ -29687,10 +29687,10 @@
         <v>1</v>
       </c>
       <c r="M123">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N123">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O123">
         <v>6</v>
@@ -29920,13 +29920,13 @@
         <v>1</v>
       </c>
       <c r="L124">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M124">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N124">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O124">
         <v>6</v>
@@ -30156,13 +30156,13 @@
         <v>12</v>
       </c>
       <c r="L125">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M125">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N125">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O125">
         <v>6</v>
@@ -30392,13 +30392,13 @@
         <v>1</v>
       </c>
       <c r="L126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N126">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O126">
         <v>6</v>
@@ -30625,7 +30625,7 @@
         <v>5</v>
       </c>
       <c r="L127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M127">
         <v>1</v>
@@ -30861,13 +30861,13 @@
         <v>1</v>
       </c>
       <c r="L128">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M128">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O128">
         <v>6</v>
@@ -31094,13 +31094,13 @@
         <v>2</v>
       </c>
       <c r="L129">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M129">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N129">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O129">
         <v>6</v>
@@ -31330,13 +31330,13 @@
         <v>3</v>
       </c>
       <c r="L130">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M130">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N130">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O130">
         <v>6</v>
@@ -31566,13 +31566,13 @@
         <v>0</v>
       </c>
       <c r="L131">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M131">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N131">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O131">
         <v>6</v>
@@ -31802,13 +31802,13 @@
         <v>2</v>
       </c>
       <c r="L132">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M132">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N132">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O132">
         <v>6</v>
@@ -32038,13 +32038,13 @@
         <v>5</v>
       </c>
       <c r="L133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O133">
         <v>6</v>
@@ -32274,13 +32274,13 @@
         <v>2</v>
       </c>
       <c r="L134">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M134">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N134">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O134">
         <v>6</v>
@@ -32510,13 +32510,13 @@
         <v>1</v>
       </c>
       <c r="L135">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M135">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N135">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O135">
         <v>6</v>
@@ -32746,13 +32746,13 @@
         <v>2</v>
       </c>
       <c r="L136">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M136">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O136">
         <v>6</v>
@@ -32982,13 +32982,13 @@
         <v>1</v>
       </c>
       <c r="L137">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N137">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O137">
         <v>6</v>
@@ -33218,13 +33218,13 @@
         <v>1</v>
       </c>
       <c r="L138">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M138">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N138">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O138">
         <v>6</v>
@@ -33454,13 +33454,13 @@
         <v>1</v>
       </c>
       <c r="L139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N139">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O139">
         <v>6</v>
@@ -33690,13 +33690,13 @@
         <v>1</v>
       </c>
       <c r="L140">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M140">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N140">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O140">
         <v>6</v>
@@ -33926,13 +33926,13 @@
         <v>1</v>
       </c>
       <c r="L141">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M141">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N141">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O141">
         <v>6</v>
@@ -34159,13 +34159,13 @@
         <v>2</v>
       </c>
       <c r="L142">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M142">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N142">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O142">
         <v>6</v>
@@ -34395,13 +34395,13 @@
         <v>2</v>
       </c>
       <c r="L143">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M143">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N143">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O143">
         <v>6</v>
@@ -34631,13 +34631,13 @@
         <v>1</v>
       </c>
       <c r="L144">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M144">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N144">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O144">
         <v>6</v>
@@ -34867,13 +34867,13 @@
         <v>3</v>
       </c>
       <c r="L145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M145">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N145">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O145">
         <v>6</v>
@@ -35103,13 +35103,13 @@
         <v>1</v>
       </c>
       <c r="L146">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M146">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N146">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O146">
         <v>6</v>
@@ -35339,13 +35339,13 @@
         <v>1</v>
       </c>
       <c r="L147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N147">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O147">
         <v>6</v>
@@ -35575,13 +35575,13 @@
         <v>1</v>
       </c>
       <c r="L148">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M148">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N148">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O148">
         <v>6</v>
@@ -35811,13 +35811,13 @@
         <v>5</v>
       </c>
       <c r="L149">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N149">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O149">
         <v>6</v>
@@ -36047,13 +36047,13 @@
         <v>3</v>
       </c>
       <c r="L150">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M150">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N150">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O150">
         <v>6</v>
@@ -36283,13 +36283,13 @@
         <v>2</v>
       </c>
       <c r="L151">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M151">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N151">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O151">
         <v>6</v>
@@ -36519,13 +36519,13 @@
         <v>3</v>
       </c>
       <c r="L152">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M152">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N152">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O152">
         <v>6</v>
@@ -36755,13 +36755,13 @@
         <v>1</v>
       </c>
       <c r="L153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O153">
         <v>6</v>
@@ -36994,7 +36994,7 @@
         <v>1</v>
       </c>
       <c r="N154">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O154">
         <v>6</v>
@@ -37224,10 +37224,10 @@
         <v>1</v>
       </c>
       <c r="L155">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M155">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N155">
         <v>1</v>
@@ -37457,10 +37457,10 @@
         <v>100</v>
       </c>
       <c r="L156">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M156">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N156">
         <v>1</v>
@@ -37693,13 +37693,13 @@
         <v>1</v>
       </c>
       <c r="L157">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M157">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N157">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O157">
         <v>6</v>
@@ -37929,13 +37929,13 @@
         <v>1</v>
       </c>
       <c r="L158">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M158">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N158">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O158">
         <v>6</v>
@@ -38162,13 +38162,13 @@
         <v>2</v>
       </c>
       <c r="L159">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M159">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N159">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O159">
         <v>6</v>
@@ -38398,13 +38398,13 @@
         <v>1</v>
       </c>
       <c r="L160">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M160">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N160">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O160">
         <v>6</v>
@@ -38634,13 +38634,13 @@
         <v>1</v>
       </c>
       <c r="L161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O161">
         <v>6</v>
@@ -38870,13 +38870,13 @@
         <v>1</v>
       </c>
       <c r="L162">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M162">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N162">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O162">
         <v>6</v>
@@ -39106,13 +39106,13 @@
         <v>5</v>
       </c>
       <c r="L163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O163">
         <v>6</v>
@@ -39342,13 +39342,13 @@
         <v>1</v>
       </c>
       <c r="L164">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M164">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N164">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O164">
         <v>6</v>
@@ -39578,13 +39578,13 @@
         <v>1</v>
       </c>
       <c r="L165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O165">
         <v>6</v>
@@ -39814,13 +39814,13 @@
         <v>1</v>
       </c>
       <c r="L166">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M166">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N166">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O166">
         <v>6</v>
@@ -40047,13 +40047,13 @@
         <v>0</v>
       </c>
       <c r="L167">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M167">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N167">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O167">
         <v>6</v>
@@ -40283,13 +40283,13 @@
         <v>1</v>
       </c>
       <c r="L168">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M168">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N168">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O168">
         <v>6</v>
@@ -40519,7 +40519,7 @@
         <v>1</v>
       </c>
       <c r="M169">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N169">
         <v>1</v>
@@ -40752,13 +40752,13 @@
         <v>5</v>
       </c>
       <c r="L170">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M170">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N170">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O170">
         <v>6</v>
@@ -40988,13 +40988,13 @@
         <v>0</v>
       </c>
       <c r="L171">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M171">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N171">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O171">
         <v>6</v>
@@ -41224,13 +41224,13 @@
         <v>0</v>
       </c>
       <c r="L172">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M172">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N172">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O172">
         <v>6</v>
@@ -41460,13 +41460,13 @@
         <v>1</v>
       </c>
       <c r="L173">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M173">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N173">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O173">
         <v>6</v>
@@ -41693,13 +41693,13 @@
         <v>5</v>
       </c>
       <c r="L174">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M174">
         <v>1</v>
       </c>
       <c r="N174">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O174">
         <v>6</v>
@@ -41926,13 +41926,13 @@
         <v>1</v>
       </c>
       <c r="L175">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M175">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N175">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O175">
         <v>6</v>
@@ -42162,13 +42162,13 @@
         <v>2</v>
       </c>
       <c r="L176">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M176">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N176">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O176">
         <v>6</v>
@@ -42870,13 +42870,13 @@
         <v>0</v>
       </c>
       <c r="L179">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M179">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N179">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O179">
         <v>6</v>
@@ -43106,13 +43106,13 @@
         <v>1</v>
       </c>
       <c r="L180">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M180">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N180">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O180">
         <v>6</v>
@@ -43342,13 +43342,13 @@
         <v>1</v>
       </c>
       <c r="L181">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M181">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N181">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O181">
         <v>6</v>
@@ -43575,13 +43575,13 @@
         <v>2</v>
       </c>
       <c r="L182">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M182">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N182">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O182">
         <v>6</v>
@@ -43808,13 +43808,13 @@
         <v>1</v>
       </c>
       <c r="L183">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M183">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N183">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O183">
         <v>6</v>

</xml_diff>